<commit_message>
I have added continue page testing script and correct the scripts
</commit_message>
<xml_diff>
--- a/Admin_panel_new2/src/test/resources/Test_Data_For_Admin.xlsx
+++ b/Admin_panel_new2/src/test/resources/Test_Data_For_Admin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7665" firstSheet="3" activeTab="6"/>
+    <workbookView windowWidth="19890" windowHeight="7665" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="38">
   <si>
     <t>username</t>
   </si>
@@ -46,6 +46,9 @@
     <t>type</t>
   </si>
   <si>
+    <t>Tenant</t>
+  </si>
+  <si>
     <t>ugadd2</t>
   </si>
   <si>
@@ -58,16 +61,13 @@
     <t>Batch@123</t>
   </si>
   <si>
+    <t>Test</t>
+  </si>
+  <si>
     <t>ugadd3</t>
   </si>
   <si>
-    <t>ugau1</t>
-  </si>
-  <si>
-    <t>ug3</t>
-  </si>
-  <si>
-    <t>ug</t>
+    <t>AlertSvc</t>
   </si>
   <si>
     <t>UserId</t>
@@ -82,9 +82,6 @@
     <t>ReEnterPassword</t>
   </si>
   <si>
-    <t>Tenant</t>
-  </si>
-  <si>
     <t>UserType</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
   </si>
   <si>
     <t>BPCode</t>
-  </si>
-  <si>
-    <t>Test</t>
   </si>
   <si>
     <t>test</t>
@@ -150,10 +144,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -185,47 +179,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -262,14 +233,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -278,6 +241,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -294,12 +272,20 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -309,6 +295,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -323,49 +317,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -377,127 +485,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -514,6 +508,45 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -542,16 +575,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -566,197 +608,149 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1122,24 +1116,24 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1154,7 +1148,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="4"/>
@@ -1172,45 +1166,47 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2"/>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="Batch@123"/>
+    <hyperlink ref="D2" r:id="rId1" display="Batch@123" tooltip="mailto:Batch@123"/>
     <hyperlink ref="D3" r:id="rId1" display="Batch@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1223,8 +1219,8 @@
   <sheetPr/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="4"/>
@@ -1246,31 +1242,31 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -1291,26 +1287,37 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1352,24 +1359,24 @@
         <v>17</v>
       </c>
       <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>21</v>
-      </c>
-      <c r="J1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2">
         <v>123456</v>
@@ -1378,30 +1385,30 @@
         <v>123456</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
         <v>25</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>123456</v>
@@ -1410,22 +1417,22 @@
         <v>123456</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
       <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
         <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1465,15 +1472,15 @@
         <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2">
         <v>123456</v>
@@ -1482,18 +1489,18 @@
         <v>123456</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>123456</v>
@@ -1502,10 +1509,10 @@
         <v>123456</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1519,7 +1526,7 @@
   <sheetPr/>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1532,12 +1539,12 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1559,44 +1566,44 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1618,35 +1625,35 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
today run script for 1300 build and did minor changes
</commit_message>
<xml_diff>
--- a/Admin_panel_new2/src/test/resources/Test_Data_For_Admin.xlsx
+++ b/Admin_panel_new2/src/test/resources/Test_Data_For_Admin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7665" activeTab="2"/>
+    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="7" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,16 @@
     <sheet name="RoleAdd" sheetId="8" r:id="rId8"/>
     <sheet name="RoleUpdate" sheetId="9" r:id="rId9"/>
     <sheet name="RoleDelete" sheetId="10" r:id="rId10"/>
+    <sheet name="AuthAdd" sheetId="11" r:id="rId11"/>
+    <sheet name="AuthUpdate" sheetId="12" r:id="rId12"/>
+    <sheet name="AuthDelete" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="42">
   <si>
     <t>username</t>
   </si>
@@ -137,6 +140,18 @@
   </si>
   <si>
     <t>CVP</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>userid</t>
+  </si>
+  <si>
+    <t>Group code</t>
+  </si>
+  <si>
+    <t>copied</t>
   </si>
 </sst>
 </file>
@@ -144,10 +159,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -173,9 +188,69 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -187,52 +262,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -241,6 +270,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -257,13 +301,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -278,28 +315,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,19 +332,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -341,163 +512,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -508,6 +523,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -550,15 +574,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -570,6 +585,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -591,15 +615,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -611,146 +626,146 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1142,6 +1157,120 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
@@ -1219,7 +1348,7 @@
   <sheetPr/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1331,7 +1460,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
+      <selection activeCell="G1" sqref="G1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>

</xml_diff>

<commit_message>
Tenant page Add,Update & Delete are done
</commit_message>
<xml_diff>
--- a/Admin_panel_new2/src/test/resources/Test_Data_For_Admin.xlsx
+++ b/Admin_panel_new2/src/test/resources/Test_Data_For_Admin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="7" activeTab="12"/>
+    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="8" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,16 @@
     <sheet name="AuthAdd" sheetId="11" r:id="rId11"/>
     <sheet name="AuthUpdate" sheetId="12" r:id="rId12"/>
     <sheet name="AuthDelete" sheetId="13" r:id="rId13"/>
+    <sheet name="AddTenant" sheetId="14" r:id="rId14"/>
+    <sheet name="UpdateTenant" sheetId="15" r:id="rId15"/>
+    <sheet name="DeleteTenant" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="49">
   <si>
     <t>username</t>
   </si>
@@ -152,6 +155,27 @@
   </si>
   <si>
     <t>copied</t>
+  </si>
+  <si>
+    <t>Tenant_name</t>
+  </si>
+  <si>
+    <t>Product_code_search_input</t>
+  </si>
+  <si>
+    <t>Assigned_count</t>
+  </si>
+  <si>
+    <t>User_code_search_input</t>
+  </si>
+  <si>
+    <t>tenant1</t>
+  </si>
+  <si>
+    <t>TDC</t>
+  </si>
+  <si>
+    <t>tenant2</t>
   </si>
 </sst>
 </file>
@@ -159,9 +183,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -188,28 +212,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -270,8 +280,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -285,31 +318,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -322,6 +339,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -332,187 +356,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,15 +547,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -574,21 +589,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -613,6 +613,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -626,15 +650,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -645,132 +669,133 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
@@ -1101,18 +1126,18 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1244,7 +1269,7 @@
   <sheetPr/>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1266,6 +1291,100 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -1283,16 +1402,16 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="4"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
@@ -1300,16 +1419,16 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
@@ -1317,16 +1436,16 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
@@ -1355,49 +1474,49 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="4"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1425,26 +1544,26 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1513,7 +1632,7 @@
       <c r="D2">
         <v>123456</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="s">
@@ -1545,7 +1664,7 @@
       <c r="D3">
         <v>123456</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F3" t="s">
@@ -1617,7 +1736,7 @@
       <c r="D2">
         <v>123456</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="s">
@@ -1637,7 +1756,7 @@
       <c r="D3">
         <v>123456</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F3" t="s">

</xml_diff>